<commit_message>
update bbwp_measures and er_crops
</commit_message>
<xml_diff>
--- a/dev/b_lu_brp_GR220707_decast_for_client.xlsx
+++ b/dev/b_lu_brp_GR220707_decast_for_client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROSG\0000.N.22. nmi packages\BedrijfsBodemWaterPlanCalculator\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E2CA24-165B-4209-9D6D-AFAB605AD3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1806316-5AF4-4570-B896-EA5FD33E2ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4559,13 +4559,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C465C-14B3-471B-8208-574D9C449604}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI464"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="U469" sqref="U469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4685,7 +4686,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>172</v>
       </c>
@@ -4793,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>174</v>
       </c>
@@ -4901,7 +4902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>175</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>176</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>212</v>
       </c>
@@ -5225,7 +5226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>229</v>
       </c>
@@ -5981,7 +5982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>239</v>
       </c>
@@ -6089,7 +6090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>240</v>
       </c>
@@ -6197,7 +6198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>241</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>242</v>
       </c>
@@ -6413,7 +6414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>243</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>244</v>
       </c>
@@ -6629,7 +6630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>246</v>
       </c>
@@ -6737,7 +6738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>247</v>
       </c>
@@ -6845,7 +6846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>249</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>256</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>257</v>
       </c>
@@ -7169,7 +7170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>258</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>259</v>
       </c>
@@ -7385,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>262</v>
       </c>
@@ -7493,7 +7494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>263</v>
       </c>
@@ -7601,7 +7602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>265</v>
       </c>
@@ -7709,7 +7710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>266</v>
       </c>
@@ -7817,7 +7818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>294</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>308</v>
       </c>
@@ -8033,7 +8034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>311</v>
       </c>
@@ -8249,7 +8250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>316</v>
       </c>
@@ -8357,7 +8358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>317</v>
       </c>
@@ -8465,7 +8466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>331</v>
       </c>
@@ -8573,7 +8574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>332</v>
       </c>
@@ -8681,7 +8682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>333</v>
       </c>
@@ -8789,7 +8790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>334</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>335</v>
       </c>
@@ -9005,7 +9006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>336</v>
       </c>
@@ -9113,7 +9114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>337</v>
       </c>
@@ -9221,7 +9222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>338</v>
       </c>
@@ -9329,7 +9330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>343</v>
       </c>
@@ -9437,7 +9438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>344</v>
       </c>
@@ -9545,7 +9546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>345</v>
       </c>
@@ -9653,7 +9654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>346</v>
       </c>
@@ -9761,7 +9762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>347</v>
       </c>
@@ -9869,7 +9870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>370</v>
       </c>
@@ -9977,7 +9978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>372</v>
       </c>
@@ -10409,7 +10410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>383</v>
       </c>
@@ -10517,7 +10518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>426</v>
       </c>
@@ -10625,7 +10626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>427</v>
       </c>
@@ -10733,7 +10734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>428</v>
       </c>
@@ -10841,7 +10842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>511</v>
       </c>
@@ -10949,7 +10950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>513</v>
       </c>
@@ -11057,7 +11058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>515</v>
       </c>
@@ -11165,7 +11166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>516</v>
       </c>
@@ -11273,7 +11274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>636</v>
       </c>
@@ -11381,7 +11382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>637</v>
       </c>
@@ -11489,7 +11490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>652</v>
       </c>
@@ -11597,7 +11598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>653</v>
       </c>
@@ -11705,7 +11706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>654</v>
       </c>
@@ -11813,7 +11814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>655</v>
       </c>
@@ -11921,7 +11922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>656</v>
       </c>
@@ -12029,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>657</v>
       </c>
@@ -12245,7 +12246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>659</v>
       </c>
@@ -12569,7 +12570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>662</v>
       </c>
@@ -12677,7 +12678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>663</v>
       </c>
@@ -12785,7 +12786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>664</v>
       </c>
@@ -12893,7 +12894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>665</v>
       </c>
@@ -13001,7 +13002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>666</v>
       </c>
@@ -13109,7 +13110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>669</v>
       </c>
@@ -13217,7 +13218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>670</v>
       </c>
@@ -13325,7 +13326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>671</v>
       </c>
@@ -13433,7 +13434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>672</v>
       </c>
@@ -13541,7 +13542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>794</v>
       </c>
@@ -13649,7 +13650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>795</v>
       </c>
@@ -13757,7 +13758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>796</v>
       </c>
@@ -13865,7 +13866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>799</v>
       </c>
@@ -13973,7 +13974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>800</v>
       </c>
@@ -14081,7 +14082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>801</v>
       </c>
@@ -14189,7 +14190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>802</v>
       </c>
@@ -14297,7 +14298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>803</v>
       </c>
@@ -14405,7 +14406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>804</v>
       </c>
@@ -14513,7 +14514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>814</v>
       </c>
@@ -14621,7 +14622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>853</v>
       </c>
@@ -14729,7 +14730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>854</v>
       </c>
@@ -14837,7 +14838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>859</v>
       </c>
@@ -14945,7 +14946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>863</v>
       </c>
@@ -15053,7 +15054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>864</v>
       </c>
@@ -15161,7 +15162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>944</v>
       </c>
@@ -15269,7 +15270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>964</v>
       </c>
@@ -15377,7 +15378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>965</v>
       </c>
@@ -15485,7 +15486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>967</v>
       </c>
@@ -15593,7 +15594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>968</v>
       </c>
@@ -15701,7 +15702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>970</v>
       </c>
@@ -15809,7 +15810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>971</v>
       </c>
@@ -15917,7 +15918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>973</v>
       </c>
@@ -16025,7 +16026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>974</v>
       </c>
@@ -16133,7 +16134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>976</v>
       </c>
@@ -16241,7 +16242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>977</v>
       </c>
@@ -16349,7 +16350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>979</v>
       </c>
@@ -16457,7 +16458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>980</v>
       </c>
@@ -16565,7 +16566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>982</v>
       </c>
@@ -16673,7 +16674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>983</v>
       </c>
@@ -16781,7 +16782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>985</v>
       </c>
@@ -16889,7 +16890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>986</v>
       </c>
@@ -16997,7 +16998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>988</v>
       </c>
@@ -17105,7 +17106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>989</v>
       </c>
@@ -17213,7 +17214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>991</v>
       </c>
@@ -17321,7 +17322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>992</v>
       </c>
@@ -17429,7 +17430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>994</v>
       </c>
@@ -17537,7 +17538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>995</v>
       </c>
@@ -17645,7 +17646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>997</v>
       </c>
@@ -17753,7 +17754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>998</v>
       </c>
@@ -17861,7 +17862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>999</v>
       </c>
@@ -17969,7 +17970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1000</v>
       </c>
@@ -18077,7 +18078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1001</v>
       </c>
@@ -18185,7 +18186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1002</v>
       </c>
@@ -18293,7 +18294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1003</v>
       </c>
@@ -18401,7 +18402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1004</v>
       </c>
@@ -18509,7 +18510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1005</v>
       </c>
@@ -18617,7 +18618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>1006</v>
       </c>
@@ -18725,7 +18726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1007</v>
       </c>
@@ -18833,7 +18834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1010</v>
       </c>
@@ -18941,7 +18942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1011</v>
       </c>
@@ -19049,7 +19050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1012</v>
       </c>
@@ -19157,7 +19158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1013</v>
       </c>
@@ -19265,7 +19266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1014</v>
       </c>
@@ -19373,7 +19374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1015</v>
       </c>
@@ -19481,7 +19482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1016</v>
       </c>
@@ -19589,7 +19590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1017</v>
       </c>
@@ -19697,7 +19698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1018</v>
       </c>
@@ -19805,7 +19806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1019</v>
       </c>
@@ -19913,7 +19914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1020</v>
       </c>
@@ -20021,7 +20022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1021</v>
       </c>
@@ -20129,7 +20130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1022</v>
       </c>
@@ -20237,7 +20238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1023</v>
       </c>
@@ -20345,7 +20346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1024</v>
       </c>
@@ -20453,7 +20454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1025</v>
       </c>
@@ -20561,7 +20562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1026</v>
       </c>
@@ -20669,7 +20670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1027</v>
       </c>
@@ -20777,7 +20778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1028</v>
       </c>
@@ -20885,7 +20886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1029</v>
       </c>
@@ -20993,7 +20994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1030</v>
       </c>
@@ -21101,7 +21102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1031</v>
       </c>
@@ -21209,7 +21210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1032</v>
       </c>
@@ -21317,7 +21318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1033</v>
       </c>
@@ -21425,7 +21426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1034</v>
       </c>
@@ -21533,7 +21534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1035</v>
       </c>
@@ -21641,7 +21642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1036</v>
       </c>
@@ -21749,7 +21750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1037</v>
       </c>
@@ -21857,7 +21858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1038</v>
       </c>
@@ -21965,7 +21966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1039</v>
       </c>
@@ -22073,7 +22074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1040</v>
       </c>
@@ -22181,7 +22182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1042</v>
       </c>
@@ -22289,7 +22290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1043</v>
       </c>
@@ -22397,7 +22398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1044</v>
       </c>
@@ -22505,7 +22506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1045</v>
       </c>
@@ -22613,7 +22614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1046</v>
       </c>
@@ -22721,7 +22722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1047</v>
       </c>
@@ -22829,7 +22830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1048</v>
       </c>
@@ -22937,7 +22938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1049</v>
       </c>
@@ -23045,7 +23046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1050</v>
       </c>
@@ -23153,7 +23154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1051</v>
       </c>
@@ -23261,7 +23262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1052</v>
       </c>
@@ -23369,7 +23370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1053</v>
       </c>
@@ -23477,7 +23478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1054</v>
       </c>
@@ -23585,7 +23586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1055</v>
       </c>
@@ -23693,7 +23694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1067</v>
       </c>
@@ -23801,7 +23802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1068</v>
       </c>
@@ -23909,7 +23910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1069</v>
       </c>
@@ -24017,7 +24018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1070</v>
       </c>
@@ -24125,7 +24126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1071</v>
       </c>
@@ -24233,7 +24234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1072</v>
       </c>
@@ -24341,7 +24342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1073</v>
       </c>
@@ -24449,7 +24450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1074</v>
       </c>
@@ -24557,7 +24558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1075</v>
       </c>
@@ -24665,7 +24666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>1076</v>
       </c>
@@ -24773,7 +24774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1077</v>
       </c>
@@ -24881,7 +24882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1078</v>
       </c>
@@ -24989,7 +24990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1079</v>
       </c>
@@ -25097,7 +25098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1080</v>
       </c>
@@ -25205,7 +25206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1081</v>
       </c>
@@ -25313,7 +25314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1082</v>
       </c>
@@ -25421,7 +25422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1083</v>
       </c>
@@ -25529,7 +25530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1084</v>
       </c>
@@ -25637,7 +25638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1085</v>
       </c>
@@ -25745,7 +25746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>1086</v>
       </c>
@@ -25853,7 +25854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>1087</v>
       </c>
@@ -25961,7 +25962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>1088</v>
       </c>
@@ -26069,7 +26070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>1089</v>
       </c>
@@ -26177,7 +26178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1090</v>
       </c>
@@ -26285,7 +26286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>1091</v>
       </c>
@@ -26393,7 +26394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1092</v>
       </c>
@@ -26501,7 +26502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>1093</v>
       </c>
@@ -26609,7 +26610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>1094</v>
       </c>
@@ -26717,7 +26718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>1095</v>
       </c>
@@ -26825,7 +26826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1096</v>
       </c>
@@ -26933,7 +26934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1097</v>
       </c>
@@ -27041,7 +27042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1098</v>
       </c>
@@ -27149,7 +27150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1099</v>
       </c>
@@ -27257,7 +27258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1100</v>
       </c>
@@ -27365,7 +27366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1570</v>
       </c>
@@ -27473,7 +27474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1574</v>
       </c>
@@ -27581,7 +27582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1575</v>
       </c>
@@ -27689,7 +27690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1697</v>
       </c>
@@ -27797,7 +27798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1698</v>
       </c>
@@ -27905,7 +27906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1869</v>
       </c>
@@ -28013,7 +28014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1870</v>
       </c>
@@ -28121,7 +28122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>1872</v>
       </c>
@@ -28229,7 +28230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1873</v>
       </c>
@@ -28337,7 +28338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>1874</v>
       </c>
@@ -28445,7 +28446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>1876</v>
       </c>
@@ -28553,7 +28554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1909</v>
       </c>
@@ -28661,7 +28662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>1910</v>
       </c>
@@ -28769,7 +28770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>1911</v>
       </c>
@@ -28877,7 +28878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1912</v>
       </c>
@@ -28985,7 +28986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>1914</v>
       </c>
@@ -29093,7 +29094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1915</v>
       </c>
@@ -29201,7 +29202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>1916</v>
       </c>
@@ -29309,7 +29310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>1917</v>
       </c>
@@ -29417,7 +29418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1918</v>
       </c>
@@ -29525,7 +29526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>1919</v>
       </c>
@@ -29633,7 +29634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1920</v>
       </c>
@@ -29741,7 +29742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>1921</v>
       </c>
@@ -29849,7 +29850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>1922</v>
       </c>
@@ -29957,7 +29958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>1923</v>
       </c>
@@ -30065,7 +30066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>1925</v>
       </c>
@@ -30173,7 +30174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1926</v>
       </c>
@@ -30281,7 +30282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>1927</v>
       </c>
@@ -30389,7 +30390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>1928</v>
       </c>
@@ -30497,7 +30498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>1929</v>
       </c>
@@ -30605,7 +30606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>1930</v>
       </c>
@@ -30713,7 +30714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>1931</v>
       </c>
@@ -30821,7 +30822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>1932</v>
       </c>
@@ -30929,7 +30930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>1933</v>
       </c>
@@ -31037,7 +31038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1934</v>
       </c>
@@ -31145,7 +31146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1935</v>
       </c>
@@ -31253,7 +31254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1936</v>
       </c>
@@ -31361,7 +31362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1940</v>
       </c>
@@ -31469,7 +31470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1949</v>
       </c>
@@ -31577,7 +31578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1950</v>
       </c>
@@ -31685,7 +31686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1959</v>
       </c>
@@ -31793,7 +31794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>2014</v>
       </c>
@@ -31901,7 +31902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>2015</v>
       </c>
@@ -32009,7 +32010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>2016</v>
       </c>
@@ -32117,7 +32118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>2017</v>
       </c>
@@ -32225,7 +32226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>2025</v>
       </c>
@@ -32333,7 +32334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>2026</v>
       </c>
@@ -32441,7 +32442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>2027</v>
       </c>
@@ -32549,7 +32550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>2029</v>
       </c>
@@ -32657,7 +32658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>2030</v>
       </c>
@@ -32765,7 +32766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>2031</v>
       </c>
@@ -32873,7 +32874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>2032</v>
       </c>
@@ -32981,7 +32982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>2033</v>
       </c>
@@ -33089,7 +33090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>2297</v>
       </c>
@@ -33197,7 +33198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>2298</v>
       </c>
@@ -33305,7 +33306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>2299</v>
       </c>
@@ -33413,7 +33414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>2300</v>
       </c>
@@ -33521,7 +33522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>2301</v>
       </c>
@@ -33629,7 +33630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>2302</v>
       </c>
@@ -33737,7 +33738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>2303</v>
       </c>
@@ -33845,7 +33846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>2304</v>
       </c>
@@ -33953,7 +33954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>2325</v>
       </c>
@@ -34061,7 +34062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>2326</v>
       </c>
@@ -34169,7 +34170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>2327</v>
       </c>
@@ -34277,7 +34278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>2328</v>
       </c>
@@ -34385,7 +34386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>2617</v>
       </c>
@@ -34493,7 +34494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>2618</v>
       </c>
@@ -34601,7 +34602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>2619</v>
       </c>
@@ -34709,7 +34710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>2620</v>
       </c>
@@ -34817,7 +34818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>2621</v>
       </c>
@@ -34925,7 +34926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>2622</v>
       </c>
@@ -35033,7 +35034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>2624</v>
       </c>
@@ -35141,7 +35142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>2625</v>
       </c>
@@ -35249,7 +35250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>2626</v>
       </c>
@@ -35357,7 +35358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>2628</v>
       </c>
@@ -35465,7 +35466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>2629</v>
       </c>
@@ -35573,7 +35574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>2630</v>
       </c>
@@ -35681,7 +35682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>2631</v>
       </c>
@@ -35789,7 +35790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>2633</v>
       </c>
@@ -35897,7 +35898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>2634</v>
       </c>
@@ -36005,7 +36006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>2635</v>
       </c>
@@ -36113,7 +36114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>2636</v>
       </c>
@@ -36221,7 +36222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>2637</v>
       </c>
@@ -36329,7 +36330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>2638</v>
       </c>
@@ -36437,7 +36438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>2639</v>
       </c>
@@ -36545,7 +36546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>2640</v>
       </c>
@@ -36653,7 +36654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>2641</v>
       </c>
@@ -36761,7 +36762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2642</v>
       </c>
@@ -36869,7 +36870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>2643</v>
       </c>
@@ -36977,7 +36978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>2644</v>
       </c>
@@ -37085,7 +37086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>2645</v>
       </c>
@@ -37193,7 +37194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>2650</v>
       </c>
@@ -37301,7 +37302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>2651</v>
       </c>
@@ -37517,7 +37518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>2653</v>
       </c>
@@ -37625,7 +37626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>2700</v>
       </c>
@@ -37733,7 +37734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>2701</v>
       </c>
@@ -37841,7 +37842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>2702</v>
       </c>
@@ -37949,7 +37950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>2703</v>
       </c>
@@ -38057,7 +38058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>2704</v>
       </c>
@@ -38165,7 +38166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>2705</v>
       </c>
@@ -38273,7 +38274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>2706</v>
       </c>
@@ -38381,7 +38382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>2707</v>
       </c>
@@ -38489,7 +38490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>2708</v>
       </c>
@@ -38597,7 +38598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>2709</v>
       </c>
@@ -38705,7 +38706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>2710</v>
       </c>
@@ -38813,7 +38814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>2711</v>
       </c>
@@ -38921,7 +38922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>2712</v>
       </c>
@@ -39029,7 +39030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>2713</v>
       </c>
@@ -39137,7 +39138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>2714</v>
       </c>
@@ -39245,7 +39246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>2715</v>
       </c>
@@ -39353,7 +39354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>2716</v>
       </c>
@@ -39461,7 +39462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>2717</v>
       </c>
@@ -39569,7 +39570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>2718</v>
       </c>
@@ -39677,7 +39678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>2719</v>
       </c>
@@ -39785,7 +39786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>2720</v>
       </c>
@@ -39893,7 +39894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>2721</v>
       </c>
@@ -40001,7 +40002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>2722</v>
       </c>
@@ -40109,7 +40110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>2723</v>
       </c>
@@ -40217,7 +40218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>2724</v>
       </c>
@@ -40325,7 +40326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>2725</v>
       </c>
@@ -40433,7 +40434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>2726</v>
       </c>
@@ -40541,7 +40542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>2727</v>
       </c>
@@ -40649,7 +40650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>2728</v>
       </c>
@@ -40757,7 +40758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>2729</v>
       </c>
@@ -40865,7 +40866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>2730</v>
       </c>
@@ -40973,7 +40974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>2731</v>
       </c>
@@ -41081,7 +41082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>2732</v>
       </c>
@@ -41189,7 +41190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>2733</v>
       </c>
@@ -41297,7 +41298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>2734</v>
       </c>
@@ -41405,7 +41406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>2735</v>
       </c>
@@ -41513,7 +41514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>2736</v>
       </c>
@@ -41621,7 +41622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>2737</v>
       </c>
@@ -41729,7 +41730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2738</v>
       </c>
@@ -41837,7 +41838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>2739</v>
       </c>
@@ -41945,7 +41946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>2740</v>
       </c>
@@ -42053,7 +42054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>2741</v>
       </c>
@@ -42161,7 +42162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>2742</v>
       </c>
@@ -42269,7 +42270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>2743</v>
       </c>
@@ -42377,7 +42378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>2744</v>
       </c>
@@ -42485,7 +42486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>2745</v>
       </c>
@@ -42593,7 +42594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>2746</v>
       </c>
@@ -42701,7 +42702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>2747</v>
       </c>
@@ -42809,7 +42810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>2748</v>
       </c>
@@ -42917,7 +42918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>2749</v>
       </c>
@@ -43025,7 +43026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>2750</v>
       </c>
@@ -43133,7 +43134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>2751</v>
       </c>
@@ -43241,7 +43242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>2752</v>
       </c>
@@ -43349,7 +43350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>2753</v>
       </c>
@@ -43457,7 +43458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>2754</v>
       </c>
@@ -43565,7 +43566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>2755</v>
       </c>
@@ -43673,7 +43674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>2756</v>
       </c>
@@ -43781,7 +43782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>2757</v>
       </c>
@@ -43889,7 +43890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>2758</v>
       </c>
@@ -43997,7 +43998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>2759</v>
       </c>
@@ -44105,7 +44106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>2760</v>
       </c>
@@ -44213,7 +44214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>2761</v>
       </c>
@@ -44321,7 +44322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>2762</v>
       </c>
@@ -44429,7 +44430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>2763</v>
       </c>
@@ -44537,7 +44538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>2764</v>
       </c>
@@ -44645,7 +44646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>2765</v>
       </c>
@@ -44753,7 +44754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>2766</v>
       </c>
@@ -44861,7 +44862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>2767</v>
       </c>
@@ -44969,7 +44970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>2768</v>
       </c>
@@ -45077,7 +45078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>2769</v>
       </c>
@@ -45185,7 +45186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2770</v>
       </c>
@@ -45293,7 +45294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>2771</v>
       </c>
@@ -45401,7 +45402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>2772</v>
       </c>
@@ -45509,7 +45510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>2773</v>
       </c>
@@ -45617,7 +45618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>2774</v>
       </c>
@@ -45725,7 +45726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>2775</v>
       </c>
@@ -45833,7 +45834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2776</v>
       </c>
@@ -45941,7 +45942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>2777</v>
       </c>
@@ -46049,7 +46050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>2778</v>
       </c>
@@ -46157,7 +46158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>2779</v>
       </c>
@@ -46265,7 +46266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>2780</v>
       </c>
@@ -46373,7 +46374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>2781</v>
       </c>
@@ -46481,7 +46482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>2782</v>
       </c>
@@ -46589,7 +46590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>2783</v>
       </c>
@@ -46697,7 +46698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>2784</v>
       </c>
@@ -46805,7 +46806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2785</v>
       </c>
@@ -46913,7 +46914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>2786</v>
       </c>
@@ -47021,7 +47022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>2787</v>
       </c>
@@ -47129,7 +47130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>2788</v>
       </c>
@@ -47237,7 +47238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>2789</v>
       </c>
@@ -47345,7 +47346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>2790</v>
       </c>
@@ -47453,7 +47454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>2791</v>
       </c>
@@ -47561,7 +47562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>2792</v>
       </c>
@@ -47669,7 +47670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>2793</v>
       </c>
@@ -47777,7 +47778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>2794</v>
       </c>
@@ -47885,7 +47886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>2795</v>
       </c>
@@ -47993,7 +47994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>2796</v>
       </c>
@@ -48101,7 +48102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>2797</v>
       </c>
@@ -48209,7 +48210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>2798</v>
       </c>
@@ -48317,7 +48318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>2799</v>
       </c>
@@ -48425,7 +48426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>2800</v>
       </c>
@@ -48533,7 +48534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>2801</v>
       </c>
@@ -48641,7 +48642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>2802</v>
       </c>
@@ -48749,7 +48750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>2951</v>
       </c>
@@ -48857,7 +48858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>3055</v>
       </c>
@@ -48965,7 +48966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>3500</v>
       </c>
@@ -49073,7 +49074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>3501</v>
       </c>
@@ -49181,7 +49182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>3502</v>
       </c>
@@ -49289,7 +49290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>3503</v>
       </c>
@@ -49397,7 +49398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>3504</v>
       </c>
@@ -49505,7 +49506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>3505</v>
       </c>
@@ -49613,7 +49614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>3506</v>
       </c>
@@ -49721,7 +49722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>3507</v>
       </c>
@@ -49829,7 +49830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>3508</v>
       </c>
@@ -49937,7 +49938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>3509</v>
       </c>
@@ -50045,7 +50046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>3510</v>
       </c>
@@ -50153,7 +50154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>3511</v>
       </c>
@@ -50261,7 +50262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>3512</v>
       </c>
@@ -50369,7 +50370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>3513</v>
       </c>
@@ -50477,7 +50478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>3514</v>
       </c>
@@ -50585,7 +50586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>3515</v>
       </c>
@@ -50693,7 +50694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>3516</v>
       </c>
@@ -50801,7 +50802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>3517</v>
       </c>
@@ -50909,7 +50910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>3518</v>
       </c>
@@ -51017,7 +51018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>3519</v>
       </c>
@@ -51125,7 +51126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>3520</v>
       </c>
@@ -51233,7 +51234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>3521</v>
       </c>
@@ -51341,7 +51342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>3522</v>
       </c>
@@ -51449,7 +51450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>3523</v>
       </c>
@@ -51557,7 +51558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>3524</v>
       </c>
@@ -51665,7 +51666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>3718</v>
       </c>
@@ -51773,7 +51774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>3719</v>
       </c>
@@ -51881,7 +51882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>3720</v>
       </c>
@@ -51989,7 +51990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>3721</v>
       </c>
@@ -52097,7 +52098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>3722</v>
       </c>
@@ -52205,7 +52206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>3730</v>
       </c>
@@ -52313,7 +52314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>3731</v>
       </c>
@@ -52421,7 +52422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>3732</v>
       </c>
@@ -52637,7 +52638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>3792</v>
       </c>
@@ -52745,7 +52746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>3801</v>
       </c>
@@ -52853,7 +52854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>3802</v>
       </c>
@@ -52961,7 +52962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>3803</v>
       </c>
@@ -53069,7 +53070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>3804</v>
       </c>
@@ -53177,7 +53178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>3805</v>
       </c>
@@ -53282,7 +53283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>3806</v>
       </c>
@@ -53390,7 +53391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>3807</v>
       </c>
@@ -53498,7 +53499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>3808</v>
       </c>
@@ -53606,7 +53607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="455" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>6520</v>
       </c>
@@ -53714,7 +53715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>6521</v>
       </c>
@@ -53822,7 +53823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="457" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>6522</v>
       </c>
@@ -53930,7 +53931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="458" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>6632</v>
       </c>
@@ -54038,7 +54039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="459" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>6636</v>
       </c>
@@ -54146,7 +54147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="460" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>7001</v>
       </c>
@@ -54254,7 +54255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="461" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>7002</v>
       </c>
@@ -54362,7 +54363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="462" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>7003</v>
       </c>
@@ -54470,7 +54471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="463" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>7004</v>
       </c>
@@ -54578,7 +54579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="464" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>7005</v>
       </c>
@@ -54687,7 +54688,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI466" xr:uid="{4E2C465C-14B3-471B-8208-574D9C449604}"/>
+  <autoFilter ref="A1:AI466" xr:uid="{4E2C465C-14B3-471B-8208-574D9C449604}">
+    <filterColumn colId="28">
+      <filters blank="1">
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH462">
     <sortCondition ref="A2:A462"/>
   </sortState>
@@ -101283,7 +101290,7 @@
   <dimension ref="A1:BC107"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -103185,12 +103192,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -103448,21 +103458,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4cc40f53-1c4d-406e-8b7f-b0d2efc65169" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="390f5cb6-d64a-4bc2-898f-27f28368359d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C33B481-E8DC-4887-BA69-781513206033}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A49155A-5C37-480F-B8DA-99586131B398}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
+    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -103488,13 +103499,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A49155A-5C37-480F-B8DA-99586131B398}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C33B481-E8DC-4887-BA69-781513206033}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4cc40f53-1c4d-406e-8b7f-b0d2efc65169"/>
-    <ds:schemaRef ds:uri="390f5cb6-d64a-4bc2-898f-27f28368359d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>